<commit_message>
Updated readVoltage in ENT_600
Using unsigned long int to increase the precision
of calculated voltage.
</commit_message>
<xml_diff>
--- a/ENT_600/VoltageScalingFactor.xlsx
+++ b/ENT_600/VoltageScalingFactor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>R1</t>
   </si>
@@ -36,6 +36,18 @@
   </si>
   <si>
     <t>SF</t>
+  </si>
+  <si>
+    <t>ADC Ref</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>Calculated Voltage 1</t>
+  </si>
+  <si>
+    <t>Calculated Voltage 2</t>
   </si>
 </sst>
 </file>
@@ -353,15 +365,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -369,7 +384,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -377,7 +392,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -386,13 +401,51 @@
         <v>1.0336485594897735E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <f>ROUND(1/B3,0)</f>
         <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>112</v>
+      </c>
+      <c r="D7">
+        <f>(B7/1024 * B6) *B4</f>
+        <v>53.046875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <f>FLOOR(B7*B4 / 1024,1) *B6</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <f>FLOOR(B7*B4*B6 /1024,1)</f>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Voltage Design calculations
</commit_message>
<xml_diff>
--- a/ENT_600/VoltageScalingFactor.xlsx
+++ b/ENT_600/VoltageScalingFactor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>R1</t>
   </si>
@@ -48,13 +48,25 @@
   </si>
   <si>
     <t>Calculated Voltage 2</t>
+  </si>
+  <si>
+    <t>Design Side</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Max Input level</t>
+  </si>
+  <si>
+    <t>Kohm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,13 +74,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -83,8 +109,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,34 +393,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
         <v>450</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -400,8 +442,17 @@
         <f>B2/(B2+B1)</f>
         <v>1.0336485594897735E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2">
+        <v>485</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -409,16 +460,41 @@
         <f>ROUND(1/B3,0)</f>
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <f>CEILING(G3/G2,1)</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <f>1/G4</f>
+        <v>1.0309278350515464E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>450</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -429,8 +505,18 @@
         <f>(B7/1024 * B6) *B4</f>
         <v>53.046875</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f>G5/(1-G5) *G6</f>
+        <v>4.6875</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -439,7 +525,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -450,5 +536,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>